<commit_message>
Actualizado datos de brix
</commit_message>
<xml_diff>
--- a/data/data_brix.xlsx
+++ b/data/data_brix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Downloads\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C73598-A1CC-4062-8C9F-0CA73428CA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{78A318A5-0BED-4B70-9A1D-0BC58E267241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DCD5E2E6-A8A7-4D7D-AE2B-1C103AE80E80}"/>
   </bookViews>
@@ -497,7 +497,7 @@
   <dimension ref="A1:H1066"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>